<commit_message>
commit 07/22 @04:33 PM
</commit_message>
<xml_diff>
--- a/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
+++ b/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>TC Name</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Your login rejected, Pl check your user_name/password.</t>
+  </si>
+  <si>
+    <t>Dashboard Welcome to BSNL Payment Portal</t>
   </si>
 </sst>
 </file>
@@ -456,13 +459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
@@ -672,10 +673,28 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B7 D7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B7">
       <formula1>$BE$2:$BE$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Browser Firefox Commit 07/24@11:24PM
</commit_message>
<xml_diff>
--- a/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
+++ b/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
@@ -459,7 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -517,7 +519,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>27</v>
@@ -543,7 +545,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>27</v>
@@ -581,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
@@ -619,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>27</v>
@@ -651,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -674,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Browser FF and Chrome Commit 07/25@03:26 AM
</commit_message>
<xml_diff>
--- a/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
+++ b/com.BSNL.WebUI.RegressionTest/src/main/resources/TestData/loginTestData.xlsx
@@ -460,7 +460,7 @@
   <dimension ref="A1:BE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -519,7 +519,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>27</v>
@@ -545,7 +545,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>27</v>
@@ -653,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -676,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>

</xml_diff>